<commit_message>
Started new project of transcripting Oracle music
</commit_message>
<xml_diff>
--- a/Music Values.xlsx
+++ b/Music Values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\root\custom-channelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C14EBA4-808A-499E-A5EF-0CD3A481F59B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32793C1B-D371-403C-AA88-9427622A569D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="1740" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5940" yWindow="2040" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
readme file, Cave, essence
</commit_message>
<xml_diff>
--- a/Music Values.xlsx
+++ b/Music Values.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\root\custom-channelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32793C1B-D371-403C-AA88-9427622A569D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D7C3E9-A001-4C2E-B3BF-2F900413E6F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5940" yWindow="2040" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="70">
   <si>
     <t>ENV</t>
   </si>
@@ -182,6 +183,60 @@
   <si>
     <t>rain</t>
   </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>2e</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Quarter</t>
+  </si>
+  <si>
+    <t>32nd</t>
+  </si>
+  <si>
+    <t>8th trip</t>
+  </si>
+  <si>
+    <t>16 trip</t>
+  </si>
+  <si>
+    <t>32 trip</t>
+  </si>
+  <si>
+    <t>4th - 32nd trip</t>
+  </si>
+  <si>
+    <t>24-2</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>12+8+2</t>
+  </si>
+  <si>
+    <t>8th + 8th trip + 32nd trip</t>
+  </si>
+  <si>
+    <t>8th + 32nd trip</t>
+  </si>
 </sst>
 </file>
 
@@ -242,7 +297,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -259,6 +314,8 @@
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -563,7 +620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -6192,4 +6249,1490 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A15453-320F-4AEB-A039-FB00CC47D3C2}">
+  <dimension ref="F1:S57"/>
+  <sheetViews>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="S44" sqref="S44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="9.140625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="L1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F2" s="11">
+        <v>16</v>
+      </c>
+      <c r="G2">
+        <f>HEX2DEC(F2)</f>
+        <v>22</v>
+      </c>
+      <c r="H2">
+        <f>SUM($G$2:G2)</f>
+        <v>22</v>
+      </c>
+      <c r="I2">
+        <f>_xlfn.FLOOR.MATH((H2/$K$2+1))</f>
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <f>H2-(I2-1)*$K$2</f>
+        <v>22</v>
+      </c>
+      <c r="K2">
+        <f>24*6</f>
+        <v>144</v>
+      </c>
+      <c r="L2">
+        <f>_xlfn.FLOOR.MATH(J2/$L$1)+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F3" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G56" si="0">HEX2DEC(F3)</f>
+        <v>12</v>
+      </c>
+      <c r="H3">
+        <f>SUM($G$2:G3)</f>
+        <v>34</v>
+      </c>
+      <c r="I3">
+        <f>_xlfn.FLOOR.MATH((H3/$K$2+1))</f>
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <f>H3-(I3-1)*$K$2</f>
+        <v>34</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L56" si="1">_xlfn.FLOOR.MATH(J3/$L$1)+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F4" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H4">
+        <f>SUM($G$2:G4)</f>
+        <v>46</v>
+      </c>
+      <c r="I4">
+        <f>_xlfn.FLOOR.MATH((H4/$K$2+1))</f>
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <f>H4-(I4-1)*$K$2</f>
+        <v>46</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F5" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H5">
+        <f>SUM($G$2:G5)</f>
+        <v>58</v>
+      </c>
+      <c r="I5">
+        <f>_xlfn.FLOOR.MATH((H5/$K$2+1))</f>
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <f>H5-(I5-1)*$K$2</f>
+        <v>58</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F6" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H6">
+        <f>SUM($G$2:G6)</f>
+        <v>70</v>
+      </c>
+      <c r="I6">
+        <f>_xlfn.FLOOR.MATH((H6/$K$2+1))</f>
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <f>H6-(I6-1)*$K$2</f>
+        <v>70</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F7" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="H7">
+        <f>SUM($G$2:G7)</f>
+        <v>84</v>
+      </c>
+      <c r="I7">
+        <f>_xlfn.FLOOR.MATH((H7/$K$2+1))</f>
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <f>H7-(I7-1)*$K$2</f>
+        <v>84</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F8" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <f>SUM($G$2:G8)</f>
+        <v>96</v>
+      </c>
+      <c r="I8">
+        <f>_xlfn.FLOOR.MATH((H8/$K$2+1))</f>
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <f>H8-(I8-1)*$K$2</f>
+        <v>96</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F9" s="11">
+        <v>18</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="H9">
+        <f>SUM($G$2:G9)</f>
+        <v>120</v>
+      </c>
+      <c r="I9">
+        <f>_xlfn.FLOOR.MATH((H9/$K$2+1))</f>
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <f>H9-(I9-1)*$K$2</f>
+        <v>120</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="H10">
+        <f>SUM($G$2:G10)</f>
+        <v>166</v>
+      </c>
+      <c r="I10">
+        <f>_xlfn.FLOOR.MATH((H10/$K$2+1))</f>
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <f>H10-(I10-1)*$K$2</f>
+        <v>22</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F11" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H11">
+        <f>SUM($G$2:G11)</f>
+        <v>178</v>
+      </c>
+      <c r="I11">
+        <f>_xlfn.FLOOR.MATH((H11/$K$2+1))</f>
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <f>H11-(I11-1)*$K$2</f>
+        <v>34</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F12" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H12">
+        <f>SUM($G$2:G12)</f>
+        <v>190</v>
+      </c>
+      <c r="I12">
+        <f>_xlfn.FLOOR.MATH((H12/$K$2+1))</f>
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <f>H12-(I12-1)*$K$2</f>
+        <v>46</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F13" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H13">
+        <f>SUM($G$2:G13)</f>
+        <v>202</v>
+      </c>
+      <c r="I13">
+        <f>_xlfn.FLOOR.MATH((H13/$K$2+1))</f>
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <f>H13-(I13-1)*$K$2</f>
+        <v>58</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F14" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H14">
+        <f>SUM($G$2:G14)</f>
+        <v>214</v>
+      </c>
+      <c r="I14">
+        <f>_xlfn.FLOOR.MATH((H14/$K$2+1))</f>
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <f>H14-(I14-1)*$K$2</f>
+        <v>70</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F15" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="H15">
+        <f>SUM($G$2:G15)</f>
+        <v>228</v>
+      </c>
+      <c r="I15">
+        <f>_xlfn.FLOOR.MATH((H15/$K$2+1))</f>
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <f>H15-(I15-1)*$K$2</f>
+        <v>84</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F16" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H16">
+        <f>SUM($G$2:G16)</f>
+        <v>240</v>
+      </c>
+      <c r="I16">
+        <f>_xlfn.FLOOR.MATH((H16/$K$2+1))</f>
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <f>H16-(I16-1)*$K$2</f>
+        <v>96</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F17" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="H17">
+        <f>SUM($G$2:G17)</f>
+        <v>264</v>
+      </c>
+      <c r="I17">
+        <f>_xlfn.FLOOR.MATH((H17/$K$2+1))</f>
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <f>H17-(I17-1)*$K$2</f>
+        <v>120</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F18" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="H18">
+        <f>SUM($G$2:G18)</f>
+        <v>310</v>
+      </c>
+      <c r="I18">
+        <f>_xlfn.FLOOR.MATH((H18/$K$2+1))</f>
+        <v>3</v>
+      </c>
+      <c r="J18">
+        <f>H18-(I18-1)*$K$2</f>
+        <v>22</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F19" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H19">
+        <f>SUM($G$2:G19)</f>
+        <v>322</v>
+      </c>
+      <c r="I19">
+        <f>_xlfn.FLOOR.MATH((H19/$K$2+1))</f>
+        <v>3</v>
+      </c>
+      <c r="J19">
+        <f>H19-(I19-1)*$K$2</f>
+        <v>34</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F20" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H20">
+        <f>SUM($G$2:G20)</f>
+        <v>334</v>
+      </c>
+      <c r="I20">
+        <f>_xlfn.FLOOR.MATH((H20/$K$2+1))</f>
+        <v>3</v>
+      </c>
+      <c r="J20">
+        <f>H20-(I20-1)*$K$2</f>
+        <v>46</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F21" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H21">
+        <f>SUM($G$2:G21)</f>
+        <v>346</v>
+      </c>
+      <c r="I21">
+        <f>_xlfn.FLOOR.MATH((H21/$K$2+1))</f>
+        <v>3</v>
+      </c>
+      <c r="J21">
+        <f>H21-(I21-1)*$K$2</f>
+        <v>58</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F22" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H22">
+        <f>SUM($G$2:G22)</f>
+        <v>358</v>
+      </c>
+      <c r="I22">
+        <f>_xlfn.FLOOR.MATH((H22/$K$2+1))</f>
+        <v>3</v>
+      </c>
+      <c r="J22">
+        <f>H22-(I22-1)*$K$2</f>
+        <v>70</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F23" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="H23">
+        <f>SUM($G$2:G23)</f>
+        <v>372</v>
+      </c>
+      <c r="I23">
+        <f>_xlfn.FLOOR.MATH((H23/$K$2+1))</f>
+        <v>3</v>
+      </c>
+      <c r="J23">
+        <f>H23-(I23-1)*$K$2</f>
+        <v>84</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F24" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H24">
+        <f>SUM($G$2:G24)</f>
+        <v>384</v>
+      </c>
+      <c r="I24">
+        <f>_xlfn.FLOOR.MATH((H24/$K$2+1))</f>
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <f>H24-(I24-1)*$K$2</f>
+        <v>96</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F25" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="H25">
+        <f>SUM($G$2:G25)</f>
+        <v>408</v>
+      </c>
+      <c r="I25">
+        <f>_xlfn.FLOOR.MATH((H25/$K$2+1))</f>
+        <v>3</v>
+      </c>
+      <c r="J25">
+        <f>H25-(I25-1)*$K$2</f>
+        <v>120</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F26" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="H26">
+        <f>SUM($G$2:G26)</f>
+        <v>454</v>
+      </c>
+      <c r="I26">
+        <f>_xlfn.FLOOR.MATH((H26/$K$2+1))</f>
+        <v>4</v>
+      </c>
+      <c r="J26">
+        <f>H26-(I26-1)*$K$2</f>
+        <v>22</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F27" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H27">
+        <f>SUM($G$2:G27)</f>
+        <v>466</v>
+      </c>
+      <c r="I27">
+        <f>_xlfn.FLOOR.MATH((H27/$K$2+1))</f>
+        <v>4</v>
+      </c>
+      <c r="J27">
+        <f>H27-(I27-1)*$K$2</f>
+        <v>34</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F28" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H28">
+        <f>SUM($G$2:G28)</f>
+        <v>478</v>
+      </c>
+      <c r="I28">
+        <f>_xlfn.FLOOR.MATH((H28/$K$2+1))</f>
+        <v>4</v>
+      </c>
+      <c r="J28">
+        <f>H28-(I28-1)*$K$2</f>
+        <v>46</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F29" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H29">
+        <f>SUM($G$2:G29)</f>
+        <v>490</v>
+      </c>
+      <c r="I29">
+        <f>_xlfn.FLOOR.MATH((H29/$K$2+1))</f>
+        <v>4</v>
+      </c>
+      <c r="J29">
+        <f>H29-(I29-1)*$K$2</f>
+        <v>58</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F30" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H30">
+        <f>SUM($G$2:G30)</f>
+        <v>502</v>
+      </c>
+      <c r="I30">
+        <f>_xlfn.FLOOR.MATH((H30/$K$2+1))</f>
+        <v>4</v>
+      </c>
+      <c r="J30">
+        <f>H30-(I30-1)*$K$2</f>
+        <v>70</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F31" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="H31">
+        <f>SUM($G$2:G31)</f>
+        <v>516</v>
+      </c>
+      <c r="I31">
+        <f>_xlfn.FLOOR.MATH((H31/$K$2+1))</f>
+        <v>4</v>
+      </c>
+      <c r="J31">
+        <f>H31-(I31-1)*$K$2</f>
+        <v>84</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F32" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H32">
+        <f>SUM($G$2:G32)</f>
+        <v>528</v>
+      </c>
+      <c r="I32">
+        <f>_xlfn.FLOOR.MATH((H32/$K$2+1))</f>
+        <v>4</v>
+      </c>
+      <c r="J32">
+        <f>H32-(I32-1)*$K$2</f>
+        <v>96</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F33" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="H33">
+        <f>SUM($G$2:G33)</f>
+        <v>552</v>
+      </c>
+      <c r="I33">
+        <f>_xlfn.FLOOR.MATH((H33/$K$2+1))</f>
+        <v>4</v>
+      </c>
+      <c r="J33">
+        <f>H33-(I33-1)*$K$2</f>
+        <v>120</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="O33">
+        <v>2</v>
+      </c>
+      <c r="P33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F34" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="H34">
+        <f>SUM($G$2:G34)</f>
+        <v>598</v>
+      </c>
+      <c r="I34">
+        <f>_xlfn.FLOOR.MATH((H34/$K$2+1))</f>
+        <v>5</v>
+      </c>
+      <c r="J34">
+        <f>H34-(I34-1)*$K$2</f>
+        <v>22</v>
+      </c>
+      <c r="K34">
+        <v>96</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>3</v>
+      </c>
+      <c r="P34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F35" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H35">
+        <f>SUM($G$2:G35)</f>
+        <v>610</v>
+      </c>
+      <c r="I35">
+        <f>_xlfn.FLOOR.MATH(((H35-$K$2*4)/$K$34+1))+4</f>
+        <v>5</v>
+      </c>
+      <c r="J35">
+        <f>H35-4*$K$2-(I35-5)*$K$34</f>
+        <v>34</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="O35">
+        <v>4</v>
+      </c>
+      <c r="P35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F36" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H36">
+        <f>SUM($G$2:G36)</f>
+        <v>622</v>
+      </c>
+      <c r="I36">
+        <f t="shared" ref="I36:I56" si="2">_xlfn.FLOOR.MATH(((H36-$K$2*4)/$K$34+1))+4</f>
+        <v>5</v>
+      </c>
+      <c r="J36">
+        <f>H36-4*$K$2-(I36-5)*$K$34</f>
+        <v>46</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="O36">
+        <v>6</v>
+      </c>
+      <c r="P36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F37" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H37">
+        <f>SUM($G$2:G37)</f>
+        <v>634</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="J37">
+        <f>H37-4*$K$2-(I37-5)*$K$34</f>
+        <v>58</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="O37">
+        <v>8</v>
+      </c>
+      <c r="P37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F38" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H38">
+        <f>SUM($G$2:G38)</f>
+        <v>646</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="J38">
+        <f>H38-4*$K$2-(I38-5)*$K$34</f>
+        <v>70</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="O38">
+        <v>12</v>
+      </c>
+      <c r="P38" t="s">
+        <v>45</v>
+      </c>
+      <c r="S38" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F39" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="H39">
+        <f>SUM($G$2:G39)</f>
+        <v>660</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="J39">
+        <f t="shared" ref="J39:J50" si="3">H39-4*$K$2-(I39-5)*$K$34</f>
+        <v>84</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="O39">
+        <v>24</v>
+      </c>
+      <c r="P39" t="s">
+        <v>57</v>
+      </c>
+      <c r="R39">
+        <v>22</v>
+      </c>
+      <c r="S39" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F40" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H40">
+        <f>SUM($G$2:G40)</f>
+        <v>672</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F41" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="H41">
+        <f>SUM($G$2:G41)</f>
+        <v>694</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S41" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F42" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H42">
+        <f>SUM($G$2:G42)</f>
+        <v>706</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F43" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H43">
+        <f>SUM($G$2:G43)</f>
+        <v>718</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="R43">
+        <v>14</v>
+      </c>
+      <c r="S43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F44" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H44">
+        <f>SUM($G$2:G44)</f>
+        <v>730</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F45" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H45">
+        <f>SUM($G$2:G45)</f>
+        <v>742</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F46" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="H46">
+        <f>SUM($G$2:G46)</f>
+        <v>756</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="3"/>
+        <v>84</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F47" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H47">
+        <f>SUM($G$2:G47)</f>
+        <v>768</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F48" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="H48">
+        <f>SUM($G$2:G48)</f>
+        <v>790</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="J48">
+        <f>H48-4*$K$2-2*$K$34-(I48-7)*$K$48</f>
+        <v>22</v>
+      </c>
+      <c r="K48">
+        <f>K34+12</f>
+        <v>108</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F49" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H49">
+        <f>SUM($G$2:G49)</f>
+        <v>802</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="J49">
+        <f t="shared" ref="J49:J56" si="4">H49-4*$K$2-2*$K$34-(I49-7)*$K$48</f>
+        <v>34</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F50" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H50">
+        <f>SUM($G$2:G50)</f>
+        <v>814</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="4"/>
+        <v>46</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F51" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H51">
+        <f>SUM($G$2:G51)</f>
+        <v>816</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F52" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H52">
+        <f>SUM($G$2:G52)</f>
+        <v>828</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F53" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H53">
+        <f>SUM($G$2:G53)</f>
+        <v>840</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="4"/>
+        <v>72</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F54" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H54">
+        <f>SUM($G$2:G54)</f>
+        <v>852</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="4"/>
+        <v>84</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F55" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H55">
+        <f>SUM($G$2:G55)</f>
+        <v>860</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="4"/>
+        <v>92</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F56" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="0"/>
+        <v>148</v>
+      </c>
+      <c r="H56">
+        <f>SUM($G$2:G56)</f>
+        <v>1008</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="J56">
+        <f>H56-4*$K$2-2*$K$34-$K$48-(I56-8)*$K$2</f>
+        <v>-12</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F57" s="10" t="str">
+        <f>DEC2HEX(G57)</f>
+        <v>3F0</v>
+      </c>
+      <c r="G57">
+        <f>SUM(G2:G56)</f>
+        <v>1008</v>
+      </c>
+      <c r="L57">
+        <f>4*K2+2*K34+K48+K2</f>
+        <v>1020</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Linebeck's Theme, wrote up music sheet for multiple songs
</commit_message>
<xml_diff>
--- a/Music Values.xlsx
+++ b/Music Values.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\root\custom-channelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE7F2CA-5A46-42D0-B45B-510D8CD04925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F2858A-292B-4739-B3E3-66124BF9053C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25920" yWindow="495" windowWidth="10920" windowHeight="12015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26280" yWindow="705" windowWidth="29040" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,13 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2261,8 +2268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84:A111"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="H89" sqref="H89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>